<commit_message>
EPBDS-1502 Added several tests.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/testmethod/UserExceptionTest.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/testmethod/UserExceptionTest.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
   <si>
     <t>C1</t>
   </si>
@@ -55,12 +55,6 @@
     <t>Expected Risk</t>
   </si>
   <si>
-    <t>Rules DoubleValue driverRiskScoreTest(String driverRisk)</t>
-  </si>
-  <si>
-    <t>Testmethod driverRiskScoreTest driverRiskTest</t>
-  </si>
-  <si>
     <t>My Exception</t>
   </si>
   <si>
@@ -74,6 +68,21 @@
   </si>
   <si>
     <t>Expected Error</t>
+  </si>
+  <si>
+    <t>=error("");0</t>
+  </si>
+  <si>
+    <t>Rules DoubleValue driverRiskScoreTest1(String driverRisk)</t>
+  </si>
+  <si>
+    <t>Rules DoubleValue driverRiskScoreTest2(String driverRisk)</t>
+  </si>
+  <si>
+    <t>Testmethod driverRiskScoreTest1 driverRiskTest1</t>
+  </si>
+  <si>
+    <t>Testmethod driverRiskScoreTest2 driverRiskTest2</t>
   </si>
 </sst>
 </file>
@@ -445,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -460,48 +469,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
@@ -514,6 +482,46 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -808,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B4:D23"/>
+  <dimension ref="B4:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -823,119 +831,203 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:4">
-      <c r="B4" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
+      <c r="B4" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="13"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="15"/>
+      <c r="C7" s="32"/>
       <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:4">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:4">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="5">
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="2:4">
-      <c r="B10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="20" t="s">
-        <v>16</v>
+      <c r="B10" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:4">
       <c r="B13" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="24"/>
+      <c r="D13" s="25"/>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="17">
+        <v>100</v>
+      </c>
+      <c r="D16" s="13"/>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="22"/>
-    </row>
-    <row r="14" spans="2:4">
-      <c r="B14" s="24" t="s">
+      <c r="C17" s="18"/>
+      <c r="D17" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="D21" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="30"/>
+      <c r="D22" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="32"/>
+      <c r="D23" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="D24" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="22"/>
+      <c r="D25" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="24"/>
+      <c r="D28" s="25"/>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C29" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="28" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15" s="25" t="s">
+      <c r="D29" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C30" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="34">
-        <v>100</v>
-      </c>
-      <c r="D16" s="30"/>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
+      <c r="D30" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="15">
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B9:C9"/>
@@ -944,9 +1036,16 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25 B10">
       <formula1>driver_type</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>